<commit_message>
bag fixed error page
</commit_message>
<xml_diff>
--- a/src/main/resources/static/doc/Template for add card.xlsx
+++ b/src/main/resources/static/doc/Template for add card.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javoh\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\AvtoPog\src\main\resources\static\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61B5EB02-E405-4874-94EF-6A3E8D87C41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA15F78F-64A4-49B9-B3F3-3C383DB1C07A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2148" yWindow="1188" windowWidth="17280" windowHeight="9420" xr2:uid="{335F8E74-3F3A-4285-85B4-15D7D5DFB36F}"/>
+    <workbookView xWindow="3192" yWindow="2232" windowWidth="17280" windowHeight="9420" xr2:uid="{335F8E74-3F3A-4285-85B4-15D7D5DFB36F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>МФО</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>муддати</t>
+  </si>
+  <si>
+    <t>0923</t>
+  </si>
+  <si>
+    <t>8600072911818810</t>
+  </si>
+  <si>
+    <t>1225</t>
+  </si>
+  <si>
+    <t>9860012110063493</t>
   </si>
 </sst>
 </file>
@@ -111,16 +123,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -438,18 +452,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D928E90-32D1-4152-A860-B0F88F41EC54}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" customWidth="1"/>
     <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="12" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -459,10 +473,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -471,16 +485,31 @@
         <v>325</v>
       </c>
       <c r="B2" s="2">
-        <v>22543</v>
-      </c>
-      <c r="C2" s="3">
-        <v>8600072911818810</v>
-      </c>
-      <c r="D2" s="3">
-        <v>923</v>
+        <v>23543</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>325</v>
+      </c>
+      <c r="B3" s="2">
+        <v>23544</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>